<commit_message>
A part of A*.
</commit_message>
<xml_diff>
--- a/Excel2FlatBuffers/ExcelTable/Scene.xlsx
+++ b/Excel2FlatBuffers/ExcelTable/Scene.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Study\UnityProject\BiuBiu\Excel2FlatBuffers\ExcelTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F4C2E73-8F2C-48D4-8836-A14EFC1FBB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A5E818-C40C-47E2-A89C-860EB438A7F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19290" yWindow="5010" windowWidth="27435" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18930" yWindow="4710" windowWidth="27435" windowHeight="13920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scene" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>skip</t>
   </si>
@@ -55,23 +55,64 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>家园场景</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Lobby/MainLobby</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>HomeLand/HomeLand</t>
-    <phoneticPr fontId="2" type="noConversion"/>
+    <t>战斗场景</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneLobby</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>SceneBattle</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>寻路网格配置</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tring</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>apConfig</t>
+    </r>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BattleMapConfig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,6 +130,14 @@
     <font>
       <sz val="9"/>
       <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -144,7 +193,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -169,6 +218,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -478,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -496,12 +554,12 @@
     <col min="9" max="9" width="38.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="1" customFormat="1" ht="42.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -514,8 +572,11 @@
       <c r="D2" s="10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E2" s="12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
@@ -526,8 +587,11 @@
       <c r="D3" s="10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="E3" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A4" s="6"/>
       <c r="B4" s="7" t="s">
         <v>6</v>
@@ -535,8 +599,11 @@
       <c r="D4" s="7" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E4" s="13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B5">
         <v>1</v>
       </c>
@@ -547,7 +614,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
       <c r="B6">
         <v>2</v>
       </c>
@@ -557,35 +624,38 @@
       <c r="D6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="E6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C7" s="8"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C8" s="9"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C9" s="8"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C10" s="8"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C12" s="9"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C13" s="9"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C14" s="9"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C15" s="9"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C16" s="9"/>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.15">
@@ -603,6 +673,6 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>